<commit_message>
Atualizado o teste de loja virtual e documentação do testes em excel
</commit_message>
<xml_diff>
--- a/DocumentacaoDosTestes/send4 testes.xlsx
+++ b/DocumentacaoDosTestes/send4 testes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rodrigoacevedo/teste/send4/DocumentacaoDoTestes/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rodrigoacevedo/teste/send4/DocumentacaoDosTestes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F91A934-A2E8-5C41-8322-6FDE8384546D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{24832EA3-0569-5642-AB37-4C843C55A52A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-50920" yWindow="-2640" windowWidth="27400" windowHeight="18660" activeTab="2" xr2:uid="{3D8C2C48-B36B-42A0-9613-76A18AE165CC}"/>
+    <workbookView xWindow="-28360" yWindow="-2880" windowWidth="27400" windowHeight="18660" activeTab="2" xr2:uid="{3D8C2C48-B36B-42A0-9613-76A18AE165CC}"/>
   </bookViews>
   <sheets>
     <sheet name="LojaPresencial-ProcessoDevoluca" sheetId="3" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="102">
   <si>
     <t>TCID</t>
   </si>
@@ -246,16 +246,117 @@
   </si>
   <si>
     <t>Validar cadastramento de devolução de  Loja Virtual</t>
+  </si>
+  <si>
+    <t>tester@send4.com.br</t>
+  </si>
+  <si>
+    <t>Na tela carregada, clicar no checkbox Selecionar todos</t>
+  </si>
+  <si>
+    <t>Selecionar a quantidade</t>
+  </si>
+  <si>
+    <t>Selecionar a Ação</t>
+  </si>
+  <si>
+    <t>Trocar</t>
+  </si>
+  <si>
+    <t>Selecionar o Motivo</t>
+  </si>
+  <si>
+    <t>Defeito na troca</t>
+  </si>
+  <si>
+    <t>Preencher o campo Como podemos Resolver?</t>
+  </si>
+  <si>
+    <t>Digite um texto</t>
+  </si>
+  <si>
+    <t>No próximo produto</t>
+  </si>
+  <si>
+    <t>No primeiro produto:</t>
+  </si>
+  <si>
+    <t>Devolver</t>
+  </si>
+  <si>
+    <t>Me arrependi</t>
+  </si>
+  <si>
+    <t>Digite outro texto</t>
+  </si>
+  <si>
+    <t>Na tela carregada, deve apresentar a oferta de devolução em Vale-Compras</t>
+  </si>
+  <si>
+    <t>Clicar no botão Deve prosseguir para a próxima tela. 30 dias</t>
+  </si>
+  <si>
+    <t>Clicar no botão Vou esperar meu dinheiro por30 dias</t>
+  </si>
+  <si>
+    <t>Na tela carregada, deve apresentar a oferta de Vale-compras + Super oferta com timer</t>
+  </si>
+  <si>
+    <t>NA tela carregada, deve apresentar o titulo Detalhes Bancários</t>
+  </si>
+  <si>
+    <t>Selecionar a opção</t>
+  </si>
+  <si>
+    <t>Não tenho conta</t>
+  </si>
+  <si>
+    <t>NA tela carregada, deve apresentar o titulo Selecione o método de devolução</t>
+  </si>
+  <si>
+    <t>Validar se o endereço está correto</t>
+  </si>
+  <si>
+    <t>Clicar no botão Selecione da Agência de Correios</t>
+  </si>
+  <si>
+    <t>Conferir os dados da seção de Dados do Cliente</t>
+  </si>
+  <si>
+    <t>Conferir os dados da seção de Produtos</t>
+  </si>
+  <si>
+    <t>Marcar o checkbox de Li e concordo...</t>
+  </si>
+  <si>
+    <t>Na tela seguinte, com a mensagem Sua solicitação foi realizada com sucesso!</t>
+  </si>
+  <si>
+    <t>Clicar em uma nota</t>
+  </si>
+  <si>
+    <t>Qualquer texto</t>
+  </si>
+  <si>
+    <t>Clicar em enviar avaliação</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -278,10 +379,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -292,8 +394,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1488,7 +1592,7 @@
   <dimension ref="A1:H115"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1497,6 +1601,7 @@
     <col min="3" max="3" width="34.6640625" style="3" customWidth="1"/>
     <col min="4" max="4" width="16.5" customWidth="1"/>
     <col min="6" max="6" width="30" style="3" customWidth="1"/>
+    <col min="7" max="7" width="17.83203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="26.5" style="3" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1570,11 +1675,17 @@
       <c r="F7" s="3" t="s">
         <v>63</v>
       </c>
+      <c r="G7">
+        <v>318</v>
+      </c>
     </row>
     <row r="8" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="F8" s="3" t="s">
         <v>64</v>
       </c>
+      <c r="G8" s="4" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="9" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="F9" s="3" t="s">
@@ -1584,15 +1695,211 @@
         <v>66</v>
       </c>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+      <c r="F10" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="F11" s="3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="F12" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="G12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="F13" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="G13" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="F14" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="G14" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+      <c r="F15" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="G15" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="F16" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="F17" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="G17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="F18" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="G18" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" ht="16" x14ac:dyDescent="0.2">
       <c r="B19" s="1"/>
-    </row>
-    <row r="30" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="F19" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="G19" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" ht="32" x14ac:dyDescent="0.2">
+      <c r="F20" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="G20" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" ht="32" x14ac:dyDescent="0.2">
+      <c r="F21" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H21" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" ht="32" x14ac:dyDescent="0.2">
+      <c r="F22" s="3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" ht="32" x14ac:dyDescent="0.2">
+      <c r="F23" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="H23" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" ht="48" x14ac:dyDescent="0.2">
+      <c r="F24" s="3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" ht="32" x14ac:dyDescent="0.2">
+      <c r="F25" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="H25" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8" ht="32" x14ac:dyDescent="0.2">
+      <c r="F26" s="3" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="F27" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="G27" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="28" spans="2:8" ht="32" x14ac:dyDescent="0.2">
+      <c r="F28" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H28" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="29" spans="2:8" ht="48" x14ac:dyDescent="0.2">
+      <c r="F29" s="3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="30" spans="2:8" ht="16" x14ac:dyDescent="0.2">
       <c r="B30" s="1"/>
-    </row>
-    <row r="38" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="F30" s="3" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="31" spans="2:8" ht="32" x14ac:dyDescent="0.2">
+      <c r="F31" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="32" spans="2:8" ht="32" x14ac:dyDescent="0.2">
+      <c r="F32" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H32" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="33" spans="2:8" ht="32" x14ac:dyDescent="0.2">
+      <c r="F33" s="3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="34" spans="2:8" ht="32" x14ac:dyDescent="0.2">
+      <c r="F34" s="3" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="35" spans="2:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="F35" s="3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="36" spans="2:8" ht="32" x14ac:dyDescent="0.2">
+      <c r="F36" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H36" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="37" spans="2:8" ht="48" x14ac:dyDescent="0.2">
+      <c r="F37" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="38" spans="2:8" ht="16" x14ac:dyDescent="0.2">
       <c r="B38" s="1"/>
-      <c r="F38" s="2"/>
+      <c r="F38" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="39" spans="2:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="F39" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="G39" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="40" spans="2:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="F40" s="3" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="52" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B52" s="1"/>
@@ -1620,6 +1927,9 @@
       <c r="F115" s="2"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G8" r:id="rId1" xr:uid="{F9CC896B-16AD-CD40-98FB-4E53F335E6B3}"/>
+  </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
</xml_diff>